<commit_message>
Made it a little better to look at
</commit_message>
<xml_diff>
--- a/docs/Risk-assessment/pinakes.xlsx
+++ b/docs/Risk-assessment/pinakes.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chalk\OneDrive\Έγγραφα\Μαθήματα CEID\Τεχνολογία Λογισμικού\προτζεκτ\Risk assessment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jpana\Documents\GitHub\MainTena\docs\Risk-assessment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD7C0A34-9D8E-4ACF-A2BF-3DF7F92964D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{538E0B14-6624-45B9-841F-78F2D7758F7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19800" windowHeight="11760" xr2:uid="{91601546-34A8-4769-826D-F6CB4E972DBB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{91601546-34A8-4769-826D-F6CB4E972DBB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -198,7 +198,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -221,11 +221,85 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -235,9 +309,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -262,7 +333,36 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -579,96 +679,96 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF817D33-3101-4CD5-A6C4-592E6891F015}">
   <dimension ref="C1:O17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="3" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" customWidth="1"/>
-    <col min="5" max="5" width="36.5703125" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" customWidth="1"/>
-    <col min="7" max="8" width="16.5703125" customWidth="1"/>
-    <col min="9" max="9" width="46.140625" customWidth="1"/>
-    <col min="10" max="10" width="12.7109375" customWidth="1"/>
-    <col min="11" max="11" width="15.42578125" customWidth="1"/>
-    <col min="12" max="12" width="14.28515625" customWidth="1"/>
-    <col min="13" max="13" width="13.5703125" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" customWidth="1"/>
+    <col min="5" max="5" width="36.5546875" customWidth="1"/>
+    <col min="6" max="6" width="12.88671875" customWidth="1"/>
+    <col min="7" max="8" width="16.5546875" customWidth="1"/>
+    <col min="9" max="9" width="46.109375" customWidth="1"/>
+    <col min="10" max="10" width="12.6640625" customWidth="1"/>
+    <col min="11" max="11" width="15.44140625" customWidth="1"/>
+    <col min="12" max="12" width="14.33203125" customWidth="1"/>
+    <col min="13" max="13" width="13.5546875" customWidth="1"/>
     <col min="15" max="15" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="3:15" x14ac:dyDescent="0.3">
       <c r="D1" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C3" s="16"/>
-      <c r="D3" s="16" t="s">
+    <row r="3" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="14"/>
+      <c r="G3" s="15"/>
+    </row>
+    <row r="4" spans="3:15" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="22" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="3:15" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C5" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-    </row>
-    <row r="4" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C4" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="16"/>
-      <c r="E4" s="5" t="s">
+      <c r="D5" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="G5" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="7" t="s">
+    </row>
+    <row r="6" spans="3:15" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C6" s="17"/>
+      <c r="D6" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="22" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C5" s="16"/>
-      <c r="D5" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="G5" s="6" t="s">
+    <row r="7" spans="3:15" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C7" s="18"/>
+      <c r="D7" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="21" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C6" s="16"/>
-      <c r="D6" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6" s="7" t="s">
+      <c r="F7" s="22" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C7" s="16"/>
-      <c r="D7" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="G7" s="7" t="s">
+      <c r="G7" s="22" t="s">
         <v>10</v>
       </c>
       <c r="K7" s="1"/>
@@ -677,21 +777,21 @@
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
     </row>
-    <row r="8" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:15" x14ac:dyDescent="0.3">
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
     </row>
-    <row r="9" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:15" x14ac:dyDescent="0.3">
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
     </row>
-    <row r="10" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:15" x14ac:dyDescent="0.3">
       <c r="C10" s="2" t="s">
         <v>31</v>
       </c>
@@ -701,14 +801,14 @@
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
     </row>
-    <row r="11" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:15" x14ac:dyDescent="0.3">
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
     </row>
-    <row r="12" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:15" x14ac:dyDescent="0.3">
       <c r="C12" s="3" t="s">
         <v>0</v>
       </c>
@@ -731,122 +831,126 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="3:15" ht="119.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:15" ht="138" x14ac:dyDescent="0.3">
       <c r="C13" s="4">
         <v>1</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="9" t="s">
+      <c r="E13" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F13" s="12" t="s">
+      <c r="F13" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="G13" s="13" t="s">
+      <c r="G13" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="H13" s="13" t="s">
+      <c r="H13" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="I13" s="10" t="s">
+      <c r="I13" s="7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="3:15" ht="115.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:15" ht="115.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C14" s="4">
         <v>2</v>
       </c>
-      <c r="D14" s="11" t="s">
+      <c r="D14" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E14" s="10" t="s">
+      <c r="E14" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F14" s="12" t="s">
+      <c r="F14" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="G14" s="14" t="s">
+      <c r="G14" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="H14" s="14" t="s">
+      <c r="H14" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="I14" s="9" t="s">
+      <c r="I14" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="3:15" ht="100.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:15" ht="100.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C15" s="4">
         <v>3</v>
       </c>
-      <c r="D15" s="11" t="s">
+      <c r="D15" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E15" s="9" t="s">
+      <c r="E15" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F15" s="12" t="s">
+      <c r="F15" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="G15" s="14" t="s">
+      <c r="G15" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="H15" s="14" t="s">
+      <c r="H15" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="I15" s="9" t="s">
+      <c r="I15" s="6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="3:15" ht="117.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:15" ht="117.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C16" s="4">
         <v>4</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="D16" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="E16" s="9" t="s">
+      <c r="E16" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="F16" s="13" t="s">
+      <c r="F16" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="G16" s="12" t="s">
+      <c r="G16" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="H16" s="13" t="s">
+      <c r="H16" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="I16" s="9" t="s">
+      <c r="I16" s="6" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="3:9" ht="126.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C17" s="15">
+    <row r="17" spans="3:9" ht="126.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C17" s="12">
         <v>5</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="D17" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E17" s="9" t="s">
+      <c r="E17" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="F17" s="12" t="s">
+      <c r="F17" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="G17" s="13" t="s">
+      <c r="G17" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="H17" s="13" t="s">
+      <c r="H17" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="I17" s="9" t="s">
+      <c r="I17" s="6" t="s">
         <v>29</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="C5:C7"/>
+  </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>